<commit_message>
setting up NYT books API
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{0146C309-D9C2-5F45-AD7C-DA34AE810872}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DE712E39-6696-4B49-90C8-475232979AE0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28340" yWindow="3960" windowWidth="23260" windowHeight="21060"/>
+    <workbookView xWindow="23800" yWindow="4240" windowWidth="27180" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="movies" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="131">
   <si>
     <t>Toy Story 3</t>
   </si>
@@ -368,16 +368,64 @@
   </si>
   <si>
     <t>Close Date</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Classic</t>
+  </si>
+  <si>
+    <t>YA Series</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>First Appearance on Best Sellers List (Published Date)</t>
+  </si>
+  <si>
+    <t>Last Appearance on Best Sellers List (Published Date)</t>
+  </si>
+  <si>
+    <t>Primary List</t>
+  </si>
+  <si>
+    <t>Paperback Nonfiction</t>
+  </si>
+  <si>
+    <t>Extra Solo Dates</t>
+  </si>
+  <si>
+    <t>Trade Fiction Paperback</t>
+  </si>
+  <si>
+    <t>Series Books</t>
+  </si>
+  <si>
+    <t>Earliest Book Publication Date (for series, first in series)</t>
+  </si>
+  <si>
+    <t>Not a best seller</t>
+  </si>
+  <si>
+    <t>See first in series</t>
+  </si>
+  <si>
+    <t>*Not a best seller, but book about movie appeared on Hardcover Advice</t>
+  </si>
+  <si>
+    <t>*Not a best seller, but book about movie appeared on Picture Books</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -513,12 +561,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -526,7 +568,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -706,6 +748,24 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF37887"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -867,13 +927,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -921,6 +991,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF37887"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1228,58 +1303,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M91"/>
+  <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="8" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1312,11 +1408,11 @@
       </c>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -1346,8 +1442,18 @@
       <c r="K3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1380,11 +1486,11 @@
       </c>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
@@ -1414,14 +1520,27 @@
       <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M5" s="11">
+        <v>38630</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="O5" s="8">
+        <v>39607</v>
+      </c>
+      <c r="P5" s="8">
+        <v>42351</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
@@ -1451,8 +1570,20 @@
       <c r="K6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L6" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="N6" t="s">
+        <v>125</v>
+      </c>
+      <c r="O6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="8">
+        <v>43373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1485,7 +1616,7 @@
       </c>
       <c r="L7"/>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1518,7 +1649,7 @@
       </c>
       <c r="L8"/>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1551,11 +1682,11 @@
       </c>
       <c r="L9"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
@@ -1585,8 +1716,26 @@
       <c r="K10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L10" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M10">
+        <v>2003</v>
+      </c>
+      <c r="N10" t="s">
+        <v>125</v>
+      </c>
+      <c r="O10" s="8">
+        <v>40265</v>
+      </c>
+      <c r="P10" s="8">
+        <v>40335</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>40607</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1619,11 +1768,11 @@
       </c>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="s">
@@ -1653,8 +1802,18 @@
       <c r="K12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1687,11 +1846,11 @@
       </c>
       <c r="L13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C14" t="s">
@@ -1721,8 +1880,18 @@
       <c r="K14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1755,7 +1924,7 @@
       </c>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1788,7 +1957,7 @@
       </c>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1821,7 +1990,7 @@
       </c>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1854,7 +2023,7 @@
       </c>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
@@ -1887,11 +2056,11 @@
       </c>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C20" t="s">
@@ -1921,8 +2090,18 @@
       <c r="K20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1955,7 +2134,7 @@
       </c>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1988,7 +2167,7 @@
       </c>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2021,11 +2200,11 @@
       </c>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C24" t="s">
@@ -2055,8 +2234,26 @@
       <c r="K24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M24" s="8">
+        <v>39705</v>
+      </c>
+      <c r="N24" t="s">
+        <v>125</v>
+      </c>
+      <c r="O24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P24" s="8">
+        <v>42358</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>42631</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2089,11 +2286,11 @@
       </c>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>5</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C26" t="s">
@@ -2123,12 +2320,22 @@
       <c r="K26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>6</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C27" t="s">
@@ -2158,8 +2365,18 @@
       <c r="K27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L27" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>7</v>
       </c>
@@ -2192,7 +2409,7 @@
       </c>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>8</v>
       </c>
@@ -2225,7 +2442,7 @@
       </c>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>9</v>
       </c>
@@ -2258,7 +2475,7 @@
       </c>
       <c r="L30"/>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>10</v>
       </c>
@@ -2291,11 +2508,11 @@
       </c>
       <c r="L31"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C32" t="s">
@@ -2325,8 +2542,18 @@
       <c r="K32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L32" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2359,7 +2586,7 @@
       </c>
       <c r="L33"/>
     </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2392,7 +2619,7 @@
       </c>
       <c r="L34"/>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2425,7 +2652,7 @@
       </c>
       <c r="L35"/>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2458,7 +2685,7 @@
       </c>
       <c r="L36"/>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6</v>
       </c>
@@ -2491,7 +2718,7 @@
       </c>
       <c r="L37"/>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>7</v>
       </c>
@@ -2524,11 +2751,11 @@
       </c>
       <c r="L38"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>8</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C39" t="s">
@@ -2558,8 +2785,18 @@
       <c r="K39" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L39" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+    </row>
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>9</v>
       </c>
@@ -2592,11 +2829,11 @@
       </c>
       <c r="L40"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>10</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C41" t="s">
@@ -2626,12 +2863,22 @@
       <c r="K41" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L41" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C42" t="s">
@@ -2661,12 +2908,27 @@
       <c r="K42" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L42" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M42" s="8">
+        <v>40911</v>
+      </c>
+      <c r="N42" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="O42" s="8">
+        <v>41322</v>
+      </c>
+      <c r="P42" s="8">
+        <v>42253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C43" t="s">
@@ -2696,8 +2958,18 @@
       <c r="K43" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L43" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2730,7 +3002,7 @@
       </c>
       <c r="L44"/>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2763,7 +3035,7 @@
       </c>
       <c r="L45"/>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2796,11 +3068,11 @@
       </c>
       <c r="L46"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>6</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C47" t="s">
@@ -2830,8 +3102,18 @@
       <c r="K47" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L47" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+    </row>
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>7</v>
       </c>
@@ -2864,7 +3146,7 @@
       </c>
       <c r="L48"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>8</v>
       </c>
@@ -2895,11 +3177,8 @@
       <c r="J49">
         <v>2014</v>
       </c>
-      <c r="K49" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>9</v>
       </c>
@@ -2932,7 +3211,7 @@
       </c>
       <c r="L50"/>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>10</v>
       </c>
@@ -2965,7 +3244,7 @@
       </c>
       <c r="L51"/>
     </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2998,7 +3277,7 @@
       </c>
       <c r="L52"/>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3031,7 +3310,7 @@
       </c>
       <c r="L53"/>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3</v>
       </c>
@@ -3064,7 +3343,7 @@
       </c>
       <c r="L54"/>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>4</v>
       </c>
@@ -3097,7 +3376,7 @@
       </c>
       <c r="L55"/>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>5</v>
       </c>
@@ -3130,7 +3409,7 @@
       </c>
       <c r="L56"/>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>6</v>
       </c>
@@ -3163,11 +3442,11 @@
       </c>
       <c r="L57"/>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>7</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C58" t="s">
@@ -3194,13 +3473,25 @@
       <c r="J58">
         <v>2015</v>
       </c>
-      <c r="L58"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K58" t="s">
+        <v>18</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>8</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C59" t="s">
@@ -3230,8 +3521,23 @@
       <c r="K59" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L59" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M59" s="8">
+        <v>41940</v>
+      </c>
+      <c r="N59" t="s">
+        <v>124</v>
+      </c>
+      <c r="O59" s="8">
+        <v>41959</v>
+      </c>
+      <c r="P59" s="8">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>9</v>
       </c>
@@ -3262,11 +3568,8 @@
       <c r="J60">
         <v>2015</v>
       </c>
-      <c r="K60" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>10</v>
       </c>
@@ -3299,7 +3602,7 @@
       </c>
       <c r="L61"/>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -3332,7 +3635,7 @@
       </c>
       <c r="L62"/>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2</v>
       </c>
@@ -3365,7 +3668,7 @@
       </c>
       <c r="L63"/>
     </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>3</v>
       </c>
@@ -3398,7 +3701,7 @@
       </c>
       <c r="L64"/>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>4</v>
       </c>
@@ -3431,11 +3734,11 @@
       </c>
       <c r="L65"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>5</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C66" t="s">
@@ -3465,8 +3768,18 @@
       <c r="K66" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L66" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M66" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+    </row>
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>6</v>
       </c>
@@ -3499,7 +3812,7 @@
       </c>
       <c r="L67"/>
     </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>7</v>
       </c>
@@ -3532,7 +3845,7 @@
       </c>
       <c r="L68"/>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>8</v>
       </c>
@@ -3565,7 +3878,7 @@
       </c>
       <c r="L69"/>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>9</v>
       </c>
@@ -3598,7 +3911,7 @@
       </c>
       <c r="L70"/>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>10</v>
       </c>
@@ -3631,7 +3944,7 @@
       </c>
       <c r="L71"/>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1</v>
       </c>
@@ -3664,7 +3977,7 @@
       </c>
       <c r="L72"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2</v>
       </c>
@@ -3695,11 +4008,8 @@
       <c r="J73">
         <v>2017</v>
       </c>
-      <c r="K73" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>3</v>
       </c>
@@ -3732,11 +4042,11 @@
       </c>
       <c r="L74"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>4</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C75" t="s">
@@ -3766,8 +4076,18 @@
       <c r="K75" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L75" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M75" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="N75" s="7"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="7"/>
+    </row>
+    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>5</v>
       </c>
@@ -3800,7 +4120,7 @@
       </c>
       <c r="L76"/>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>6</v>
       </c>
@@ -3833,11 +4153,11 @@
       </c>
       <c r="L77"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>7</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="7" t="s">
         <v>94</v>
       </c>
       <c r="C78" t="s">
@@ -3867,8 +4187,23 @@
       <c r="K78" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L78" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M78">
+        <v>1986</v>
+      </c>
+      <c r="N78" t="s">
+        <v>124</v>
+      </c>
+      <c r="O78" s="8">
+        <v>42981</v>
+      </c>
+      <c r="P78" s="8">
+        <v>43114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>8</v>
       </c>
@@ -3901,7 +4236,7 @@
       </c>
       <c r="L79"/>
     </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>9</v>
       </c>
@@ -3934,7 +4269,7 @@
       </c>
       <c r="L80"/>
     </row>
-    <row r="81" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>10</v>
       </c>
@@ -3965,8 +4300,9 @@
       <c r="J81">
         <v>2017</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L81"/>
+    </row>
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1</v>
       </c>
@@ -3997,8 +4333,9 @@
       <c r="J82">
         <v>2018</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L82"/>
+    </row>
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2</v>
       </c>
@@ -4029,8 +4366,9 @@
       <c r="J83">
         <v>2018</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L83"/>
+    </row>
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>3</v>
       </c>
@@ -4061,8 +4399,9 @@
       <c r="J84">
         <v>2018</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L84"/>
+    </row>
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>4</v>
       </c>
@@ -4093,8 +4432,9 @@
       <c r="J85">
         <v>2018</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L85"/>
+    </row>
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>5</v>
       </c>
@@ -4125,8 +4465,9 @@
       <c r="J86">
         <v>2018</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L86"/>
+    </row>
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>6</v>
       </c>
@@ -4157,8 +4498,9 @@
       <c r="J87">
         <v>2018</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L87"/>
+    </row>
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>7</v>
       </c>
@@ -4189,8 +4531,9 @@
       <c r="J88">
         <v>2018</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L88"/>
+    </row>
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>8</v>
       </c>
@@ -4221,8 +4564,9 @@
       <c r="J89">
         <v>2018</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L89"/>
+    </row>
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>9</v>
       </c>
@@ -4253,8 +4597,9 @@
       <c r="J90">
         <v>2018</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L90"/>
+    </row>
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>10</v>
       </c>
@@ -4285,9 +4630,10 @@
       <c r="J91">
         <v>2018</v>
       </c>
+      <c r="L91"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K91">
+  <autoFilter ref="A1:K91" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="10">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>

</xml_diff>

<commit_message>
halfway through hunger games data
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindsayhuth/Documents/GitHub/movies-and-their-books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DE712E39-6696-4B49-90C8-475232979AE0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A848115-8714-034E-9618-6A6E96F857DF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23800" yWindow="4240" windowWidth="27180" windowHeight="21060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="460" windowWidth="27180" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="movies" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">movies!$A$1:$K$91</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="131">
   <si>
     <t>Toy Story 3</t>
   </si>
@@ -927,7 +927,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -944,6 +944,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1307,8 +1308,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2243,8 +2244,8 @@
       <c r="N24" t="s">
         <v>125</v>
       </c>
-      <c r="O24" t="s">
-        <v>77</v>
+      <c r="O24" s="12">
+        <v>40433</v>
       </c>
       <c r="P24" s="8">
         <v>42358</v>

</xml_diff>

<commit_message>
built httyd + it
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lindsayhuth/Documents/GitHub/movies-and-their-books/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lhuth/Documents/GitHub/movies-and-their-books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A848115-8714-034E-9618-6A6E96F857DF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{743BC72D-AB27-304B-B485-161728E2A8D4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="460" windowWidth="27180" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">movies!$A$1:$K$91</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1309,7 +1309,7 @@
   <dimension ref="A1:Q91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1720,8 +1720,8 @@
       <c r="L10" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="M10">
-        <v>2003</v>
+      <c r="M10" s="8">
+        <v>37653</v>
       </c>
       <c r="N10" t="s">
         <v>125</v>

</xml_diff>